<commit_message>
Fully implemented the excel to csv converter for the tester
</commit_message>
<xml_diff>
--- a/unit_tester/test_files/tokenization_echo.xlsx
+++ b/unit_tester/test_files/tokenization_echo.xlsx
@@ -3245,6 +3245,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3414,10 +3415,10 @@
   <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.11"/>

</xml_diff>